<commit_message>
fixed formatting issue in grants section
</commit_message>
<xml_diff>
--- a/data/mch_cv_data.xlsx
+++ b/data/mch_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mainahandmaker/Desktop/Website:CV/mch_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A39267-311A-F84C-B110-8E2CD859494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA866C05-D41C-EC48-890D-1B0DF01CFCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19980" activeTab="9" xr2:uid="{E332C97D-16A1-8846-9B40-FA3DC448712E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="3" xr2:uid="{E332C97D-16A1-8846-9B40-FA3DC448712E}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="4" r:id="rId1"/>
@@ -177,12 +177,6 @@
     <t>Hesse Research Award</t>
   </si>
   <si>
-    <t>*PI*</t>
-  </si>
-  <si>
-    <t>*Co-PI*</t>
-  </si>
-  <si>
     <t>Atlantic Flyway Shorebird Initiative Grant</t>
   </si>
   <si>
@@ -267,24 +261,6 @@
     <t>National Science Foundation ($138,000)</t>
   </si>
   <si>
-    <t>American Ornithological Society ($2,420, *PI*)</t>
-  </si>
-  <si>
-    <t>National Fish and Wildlife Foundation ($90,000, *Co-PI*)</t>
-  </si>
-  <si>
-    <t>Association of Field Ornithologists ($1,476, *PI*)</t>
-  </si>
-  <si>
-    <t>Georgia Ornithological Society ($7,500 *PI*)</t>
-  </si>
-  <si>
-    <t>National Fish and Wildlife Foundation ($84,418 *Co-PI*)</t>
-  </si>
-  <si>
-    <t>Carolina Bird Club ($7,500, *PI*)</t>
-  </si>
-  <si>
     <t>Thunder Bay, Ontario, Canada</t>
   </si>
   <si>
@@ -435,9 +411,6 @@
     <t>Columbia, South Carolina</t>
   </si>
   <si>
-    <t>Advisor: Dr. Nathan Senner (Lab transferred institutions in Fall 2020)</t>
-  </si>
-  <si>
     <t>Marine Data Science in R</t>
   </si>
   <si>
@@ -526,6 +499,33 @@
   </si>
   <si>
     <t>2022-Present</t>
+  </si>
+  <si>
+    <t>Advisor: Dr. Nathan Senner (Lab transferred institutions in Fall 2022)</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Co-PI</t>
+  </si>
+  <si>
+    <t>American Ornithological Society ($2,420, PI)</t>
+  </si>
+  <si>
+    <t>National Fish and Wildlife Foundation ($90,000, Co-PI)</t>
+  </si>
+  <si>
+    <t>Association of Field Ornithologists ($1,476, PI)</t>
+  </si>
+  <si>
+    <t>Georgia Ornithological Society ($7,500, PI)</t>
+  </si>
+  <si>
+    <t>National Fish and Wildlife Foundation ($84,418 Co-PI)</t>
+  </si>
+  <si>
+    <t>Carolina Bird Club ($7,500, PI)</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -598,12 +598,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -923,7 +917,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -973,7 +967,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -987,19 +981,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1025,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71ED5780-55CD-9C4C-8D19-4B8553888D5F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1042,87 +1036,87 @@
         <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>122</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1148,65 +1142,65 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
         <v>139</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1335,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D2" s="5">
         <v>2020</v>
@@ -1361,13 +1355,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>30</v>
@@ -1381,13 +1375,13 @@
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>33</v>
@@ -1401,13 +1395,13 @@
         <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>36</v>
@@ -1422,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680F533E-1D11-2B48-873D-3BFD60EBCD70}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1431,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>37</v>
@@ -1454,21 +1448,21 @@
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>
@@ -1479,10 +1473,10 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>42</v>
@@ -1491,69 +1485,69 @@
         <v>2420</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="7">
         <v>90000</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="7">
         <v>1476</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>157</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7">
         <v>7500</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="7">
         <v>138000</v>
@@ -1561,58 +1555,58 @@
     </row>
     <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7">
         <v>84418</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7">
         <v>7500</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1664,16 +1658,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -1681,89 +1675,89 @@
     </row>
     <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3">
         <v>2022</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C3" s="8">
         <v>2022</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3">
         <v>2022</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3">
         <v>2021</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C6" s="3">
         <v>2021</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3">
         <v>2021</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1794,10 +1788,10 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1805,67 +1799,67 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1888,10 +1882,10 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1899,30 +1893,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dissertation fieldwork grant
</commit_message>
<xml_diff>
--- a/data/mch_cv_data.xlsx
+++ b/data/mch_cv_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mainahandmaker/Desktop/Website:CV/mch_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACD7439-5CCC-E94C-A4EF-05EA664865B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527235F-4496-1948-972C-71CF948D38D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="3" xr2:uid="{E332C97D-16A1-8846-9B40-FA3DC448712E}"/>
   </bookViews>
@@ -531,10 +531,10 @@
     <t>December 2022</t>
   </si>
   <si>
-    <t>University of Massachusetts Amherst Graduate School</t>
-  </si>
-  <si>
     <t>Dissertation Fieldwork Grant</t>
+  </si>
+  <si>
+    <t>University of Massachusetts Amherst Graduate School ($4,950)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,15 +607,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1435,7 +1426,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1464,17 +1455,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="11">
+      <c r="D2" s="7">
         <v>4950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to PhD candidate and added 2023 publications
</commit_message>
<xml_diff>
--- a/data/mch_cv_data.xlsx
+++ b/data/mch_cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mainahandmaker/Desktop/Website:CV/mch_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B527235F-4496-1948-972C-71CF948D38D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623EC609-A7F1-DE4E-9E93-B685BDEA9189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="3" xr2:uid="{E332C97D-16A1-8846-9B40-FA3DC448712E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="7" xr2:uid="{E332C97D-16A1-8846-9B40-FA3DC448712E}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="173">
   <si>
     <t>degree</t>
   </si>
@@ -171,9 +171,6 @@
     <t>American Ornithological Society</t>
   </si>
   <si>
-    <t>Travel Award to attend 2022 Annual Meeting in San Juan, Puerto Rico</t>
-  </si>
-  <si>
     <t>Hesse Research Award</t>
   </si>
   <si>
@@ -534,7 +531,40 @@
     <t>Dissertation Fieldwork Grant</t>
   </si>
   <si>
-    <t>University of Massachusetts Amherst Graduate School ($4,950)</t>
+    <t>UMass Amherst - Graduate School ($4,950)</t>
+  </si>
+  <si>
+    <t>Travel Grant</t>
+  </si>
+  <si>
+    <t>UMass Amherst - Dept. of Environmental Conservation ($200)</t>
+  </si>
+  <si>
+    <t>Travel Award</t>
+  </si>
+  <si>
+    <t>May 2023</t>
+  </si>
+  <si>
+    <t>Donald L Mader Natural Resources Conservation Award</t>
+  </si>
+  <si>
+    <t>UMass Amherst - Dept. of Environmental Conservation ($1,000)</t>
+  </si>
+  <si>
+    <t>Spring and Fall 2016</t>
+  </si>
+  <si>
+    <t>Support Staff</t>
+  </si>
+  <si>
+    <t>Tropical Biology and Conservation</t>
+  </si>
+  <si>
+    <t>UCEAP</t>
+  </si>
+  <si>
+    <t>Assisted with field instruciton and logistics for undergraduates enrolled in University of California Educaiton Abroad Program's Tropical Biology and Conservation course based in Monteverde, Costa Rica. </t>
   </si>
 </sst>
 </file>
@@ -627,7 +657,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -915,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -959,7 +989,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -976,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -990,19 +1020,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
         <v>118</v>
-      </c>
-      <c r="B4" t="s">
-        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1045,87 +1075,87 @@
         <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1151,65 +1181,65 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1374,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="5">
         <v>2020</v>
@@ -1364,13 +1394,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>30</v>
@@ -1384,13 +1414,13 @@
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>33</v>
@@ -1404,13 +1434,13 @@
         <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>36</v>
@@ -1423,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680F533E-1D11-2B48-873D-3BFD60EBCD70}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1440,7 +1470,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>37</v>
@@ -1455,181 +1485,209 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D2" s="7">
-        <v>4950</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="D7" s="7">
+        <v>2420</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="7">
-        <v>2420</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="D8" s="7">
         <v>90000</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1476</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="7">
-        <v>7500</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D9" s="7">
-        <v>138000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>1476</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7">
-        <v>84418</v>
+        <v>7500</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>159</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D11" s="7">
-        <v>7500</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>152</v>
+        <v>138000</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>157</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7">
+        <v>84418</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="D13" s="7">
+        <v>7500</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1665,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F78BAA-7D3C-C943-9715-162DED65F76A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1681,16 +1739,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -1698,89 +1756,89 @@
     </row>
     <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C2" s="3">
         <v>2022</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C3" s="8">
         <v>2022</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3">
         <v>2022</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3">
         <v>2021</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="C6" s="3">
         <v>2021</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C7" s="3">
         <v>2021</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1790,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E52EB4-B156-6A4B-B711-A8E2EAE2B821}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L20:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1811,10 +1869,10 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1822,67 +1880,84 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="D2" t="s">
-        <v>90</v>
-      </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
         <v>91</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
       <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" t="s">
-        <v>98</v>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1905,10 +1980,10 @@
         <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1916,30 +1991,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>101</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>